<commit_message>
update Key number and reports
</commit_message>
<xml_diff>
--- a/Local/Data/Export/KeyNum-Report_fhirTestData_2020.xlsx
+++ b/Local/Data/Export/KeyNum-Report_fhirTestData_2020.xlsx
@@ -20,25 +20,25 @@
     <t xml:space="preserve">report_year</t>
   </si>
   <si>
-    <t xml:space="preserve">orphaCoding_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">orphaCase_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unique_rdCase_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rdCase_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">case_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patient_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inpatientCases_no</t>
+    <t xml:space="preserve">orphaCoding_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orphaCase_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unambigous_rdCase_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdCase_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">case_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patient_no_py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">case_no_py_ipat</t>
   </si>
   <si>
     <t xml:space="preserve">260123451-Airolo</t>
@@ -410,22 +410,22 @@
         <v>2020</v>
       </c>
       <c r="C2" t="n">
-        <v>124</v>
+        <v>92</v>
       </c>
       <c r="D2" t="n">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="E2" t="n">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="F2" t="n">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="G2" t="n">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="H2" t="n">
-        <v>962</v>
+        <v>950</v>
       </c>
       <c r="I2" t="n">
         <v>10000</v>

</xml_diff>